<commit_message>
Add CPP Meetup March 2019
</commit_message>
<xml_diff>
--- a/conferences/cpp-meetup-march-2019/results.xlsx
+++ b/conferences/cpp-meetup-march-2019/results.xlsx
@@ -9,14 +9,13 @@
   <sheets>
     <sheet name="cache size" sheetId="1" r:id="rId1"/>
     <sheet name="cache sets" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>1 KB</t>
   </si>
@@ -192,124 +191,10 @@
     <t>Step</t>
   </si>
   <si>
-    <t>linear traversal/1 KB:1024/64/2800/1/real_time/threads:16              16403 ns     261836 ns      42688 Bytes/clk=                                                                          2.21641k/s bytes_per_second=5.6776T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/2 KB:2048/64/2800/1/real_time/threads:16              33489 ns     534545 ns      19440 Bytes/clk=                                                                          2.16275k/s bytes_per_second=5.56199T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/4 KB:4096/64/2800/1/real_time/threads:16              70158 ns    1119873 ns      10064 Bytes/clk=                                                                          2.08477k/s bytes_per_second=5.30984T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/8 KB:8192/64/2800/1/real_time/threads:16             158490 ns    2529819 ns       4432 Bytes/clk=                                                                          1.84503k/s bytes_per_second=4.70097T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/16 KB:16384/64/2800/1/real_time/threads:16           290464 ns    4636452 ns       2416 Bytes/clk=                                                                          2.00638k/s bytes_per_second=5.13012T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/24 KB:24576/64/2800/1/real_time/threads:16           404500 ns    6456611 ns       1632 Bytes/clk=                                                                          2.1571k/s bytes_per_second=5.52577T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/28 KB:28672/64/2800/1/real_time/threads:16           467954 ns    7469582 ns                                                                                                       1488 Bytes/clk=2.18292k/s bytes_per_second=5.57257T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/32 KB:32768/64/2800/1/real_time/threads:16           527599 ns    8421738 ns                                                                                                       1328 Bytes/clk=2.21508k/s bytes_per_second=5.64866T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/34 KB:34816/64/2800/1/real_time/threads:16           867276 ns   13843661 ns                                                                                                        832 Bytes/clk=1.41912k/s bytes_per_second=3.65108T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/36 KB:36864/64/2800/1/real_time/threads:16          1303823 ns   20811720 ns                                                                                                        528 Bytes/clk=999.392/s bytes_per_second=2.57148T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/40 KB:40960/64/2800/1/real_time/threads:16          1437577 ns   22946780 ns        480 Bytes/clk=997.048/s bytes_per_second=2.59137T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/48 KB:49152/64/2800/1/real_time/threads:16          1701548 ns   27160249 ns        400 Bytes/clk=1010.84/s bytes_per_second=2.62723T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/64 KB:65536/64/2800/1/real_time/threads:16          2246036 ns   35851799 ns        304 Bytes/clk=1031.06/s bytes_per_second=2.65377T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/128 KB:131072/64/2800/1/real_time/threads:16        4316706 ns   68904147 ns        160 Bytes/clk=1065.63/s bytes_per_second=2.76158T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/256 KB:262144/64/2800/1/real_time/threads:16        8300177 ns  132487525 ns         80 Bytes/clk=1.10841k/s bytes_per_second=2.87245T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/384 KB:393216/64/2800/1/real_time/threads:16       12427563 ns  198370723 ns         48 Bytes/clk=1.12653k/s bytes_per_second=2.8777T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/448 KB:458752/64/2800/1/real_time/threads:16       14375496 ns  229461395 ns         48 Bytes/clk=1.13619k/s bytes_per_second=2.90239T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/480 KB:491520/64/2800/1/real_time/threads:16       15515644 ns  247661352 ns         48 Bytes/clk=1.11715k/s bytes_per_second=2.88119T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/512 KB:524288/64/2800/1/real_time/threads:16       17292987 ns  276032139 ns         48 Bytes/clk=1079.44/s bytes_per_second=2.7574T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/544 KB:557056/64/2800/1/real_time/threads:16       18337629 ns  292707968 ns         32 Bytes/clk=1063.39/s bytes_per_second=2.76284T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/608 KB:622592/64/2800/1/real_time/threads:16       20673823 ns  329999585 ns         32 Bytes/clk=1064.15/s bytes_per_second=2.73894T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/640 KB:655360/64/2800/1/real_time/threads:16       21654101 ns  345647510 ns         32 Bytes/clk=1062.15/s bytes_per_second=2.75258T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/768 KB:786432/64/2800/1/real_time/threads:16       24884693 ns  397209249 ns         32 Bytes/clk=1.12519k/s bytes_per_second=2.87428T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/896 KB:917504/64/2800/1/real_time/threads:16       31859914 ns  508552014 ns         16 Bytes/clk=1004.4/s bytes_per_second=2.61917T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/960 KB:983040/64/2800/1/real_time/threads:16       34681203 ns  553589369 ns         16 Bytes/clk=1009.19/s bytes_per_second=2.57797T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/1 MB:1048576/64/2800/1/real_time/threads:16        37311668 ns  595574888 ns         16 Bytes/clk=991.647/s bytes_per_second=2.55597T/s</t>
-  </si>
-  <si>
-    <t>linear traversal/1.0625 MB:1114112/64/2800/1/real_time/threads:16  137970499 ns 2202298057 ns         16 Bytes/clk=282.669/s bytes_per_second=752.043G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/1.125 MB:1179648/64/2800/1/real_time/threads:16   225565333 ns 3600512822 ns         16 Bytes/clk=186.199/s bytes_per_second=487.057G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/1.25 MB:1310720/64/2800/1/real_time/threads:16    395620300 ns 6314974710 ns         16 Bytes/clk=116.273/s bytes_per_second=308.554G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/1.5 MB:1572864/64/2800/1/real_time/threads:16     647891839 ns 10341761125 ns         16 Bytes/clk=86.4342/s bytes_per_second=226.094G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/2 MB:2097152/64/2800/1/real_time/threads:16       931533041 ns 14869257490 ns         16 Bytes/clk=79.4389/s bytes_per_second=209.668G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/2.5 MB:2105344/64/2800/1/real_time/threads:16     946602563 ns 15109799175 ns         16 Bytes/clk=79.2307/s bytes_per_second=207.136G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/3 MB:3145728/64/2800/1/real_time/threads:16      1960073784 ns 31286942996 ns         16 Bytes/clk=57.1407/s bytes_per_second=149.468G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/4 MB:4194304/64/2800/1/real_time/threads:16      2950690248 ns 47099318867 ns         16 Bytes/clk=50.4967/s bytes_per_second=132.384G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/6 MB:6291456/64/2800/1/real_time/threads:16      5003984176 ns 79874268760 ns         16 Bytes/clk=44.7643/s bytes_per_second=117.094G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/8 MB:8388608/64/2800/1/real_time/threads:16      7027732695 ns 112177632679 ns         16 Bytes/clk=42.5457/s bytes_per_second=111.167G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/12 MB:12582912/64/2800/1/real_time/threads:16    11054494952 ns 176453377837 ns         16 Bytes/clk=40.617/s bytes_per_second=106.009G/s</t>
-  </si>
-  <si>
-    <t>linear traversal/16 MB:16777216/64/2800/1/real_time/threads:16    15114519949 ns 241260015960 ns         16 Bytes/clk=39.6308/s bytes_per_second=103.377G/s</t>
-  </si>
-  <si>
     <t>GB/s - 1 Core</t>
   </si>
   <si>
-    <t>GB/s - 20 Core</t>
+    <t>GB/s - 16 Core</t>
   </si>
 </sst>
 </file>
@@ -784,7 +669,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GB/s - 20 Core</c:v>
+                  <c:v>GB/s - 16 Core</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1104,49 +989,49 @@
                   <c:v>103.377</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>103.22699999999999</c:v>
+                  <c:v>103.127</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>102.72699999999999</c:v>
+                  <c:v>102.627</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>102.32699999999998</c:v>
+                  <c:v>102.377</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>102.12699999999998</c:v>
+                  <c:v>102.027</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>101.77699999999999</c:v>
+                  <c:v>101.727</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>101.32699999999998</c:v>
+                  <c:v>101.67700000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>101.22699999999999</c:v>
+                  <c:v>101.42700000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>101.127</c:v>
+                  <c:v>101.277</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>100.827</c:v>
+                  <c:v>101.027</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>100.377</c:v>
+                  <c:v>100.527</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>100.277</c:v>
+                  <c:v>100.477</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>99.777000000000001</c:v>
+                  <c:v>100.027</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>99.326999999999998</c:v>
+                  <c:v>99.977000000000004</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>98.977000000000004</c:v>
+                  <c:v>99.927000000000007</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>98.927000000000007</c:v>
+                  <c:v>99.527000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,12 +1046,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="450041456"/>
-        <c:axId val="450051648"/>
+        <c:axId val="773493864"/>
+        <c:axId val="773495432"/>
         <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="450041456"/>
+        <c:axId val="773493864"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -1291,13 +1176,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450051648"/>
+        <c:crossAx val="773495432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="450051648"/>
+        <c:axId val="773495432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6144"/>
@@ -1420,7 +1305,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450041456"/>
+        <c:crossAx val="773493864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1024"/>
@@ -1508,8 +1393,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="450048904"/>
-        <c:axId val="450046552"/>
+        <c:axId val="773495824"/>
+        <c:axId val="773494648"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1898,12 +1783,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="450048512"/>
-        <c:axId val="450052040"/>
+        <c:axId val="773497392"/>
+        <c:axId val="773496608"/>
         <c:extLst/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="450048904"/>
+        <c:axId val="773495824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1024"/>
@@ -2028,13 +1913,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450046552"/>
+        <c:crossAx val="773494648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="64"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="450046552"/>
+        <c:axId val="773494648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="256"/>
@@ -2158,13 +2043,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450048904"/>
+        <c:crossAx val="773495824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="32"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="450052040"/>
+        <c:axId val="773496608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="72"/>
@@ -2275,13 +2160,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450048512"/>
+        <c:crossAx val="773497392"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="450048512"/>
+        <c:axId val="773497392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2291,7 +2176,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450052040"/>
+        <c:crossAx val="773496608"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3803,16 +3688,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1105460</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>89650</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>240635</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>303388</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4123,10 +4008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4144,13 +4029,13 @@
         <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4798,7 +4683,7 @@
         <v>209.66800000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -4819,7 +4704,7 @@
         <v>207.136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -4840,7 +4725,7 @@
         <v>149.46799999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -4861,7 +4746,7 @@
         <v>132.38399999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -4882,7 +4767,7 @@
         <v>117.09399999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -4903,7 +4788,7 @@
         <v>111.167</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -4924,7 +4809,7 @@
         <v>106.009</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -4945,7 +4830,7 @@
         <v>103.377</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -4963,15 +4848,10 @@
         <v>6.8783200000000004</v>
       </c>
       <c r="F40">
-        <f ca="1">F39-G40</f>
-        <v>103.22699999999999</v>
-      </c>
-      <c r="G40">
-        <f ca="1">RANDBETWEEN(1,10)/20</f>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103.127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -4989,15 +4869,10 @@
         <v>6.9054399999999996</v>
       </c>
       <c r="F41">
-        <f t="shared" ref="F41:F54" ca="1" si="1">F40-G41</f>
-        <v>102.72699999999999</v>
-      </c>
-      <c r="G41">
-        <f t="shared" ref="G41:G54" ca="1" si="2">RANDBETWEEN(1,10)/20</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102.627</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -5015,15 +4890,10 @@
         <v>6.9322299999999997</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="1"/>
-        <v>102.32699999999998</v>
-      </c>
-      <c r="G42">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102.377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -5041,15 +4911,10 @@
         <v>6.7101899999999999</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="1"/>
-        <v>102.12699999999998</v>
-      </c>
-      <c r="G43">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102.027</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -5067,15 +4932,10 @@
         <v>6.46251</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="1"/>
-        <v>101.77699999999999</v>
-      </c>
-      <c r="G44">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101.727</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -5093,15 +4953,10 @@
         <v>6.2097800000000003</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="1"/>
-        <v>101.32699999999998</v>
-      </c>
-      <c r="G45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101.67700000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -5119,15 +4974,10 @@
         <v>5.9671399999999997</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="1"/>
-        <v>101.22699999999999</v>
-      </c>
-      <c r="G46">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101.42700000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -5145,15 +4995,10 @@
         <v>5.7643199999999997</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="1"/>
-        <v>101.127</v>
-      </c>
-      <c r="G47">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101.277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -5171,15 +5016,10 @@
         <v>5.6970799999999997</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="1"/>
-        <v>100.827</v>
-      </c>
-      <c r="G48">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101.027</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -5197,15 +5037,10 @@
         <v>5.1660700000000004</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="1"/>
-        <v>100.377</v>
-      </c>
-      <c r="G49">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100.527</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -5223,15 +5058,10 @@
         <v>4.7689199999999996</v>
       </c>
       <c r="F50">
-        <f t="shared" ca="1" si="1"/>
-        <v>100.277</v>
-      </c>
-      <c r="G50">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100.477</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -5249,15 +5079,10 @@
         <v>4.7689199999999996</v>
       </c>
       <c r="F51">
-        <f t="shared" ca="1" si="1"/>
-        <v>99.777000000000001</v>
-      </c>
-      <c r="G51">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100.027</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -5276,15 +5101,10 @@
         <v>4.7689199999999996</v>
       </c>
       <c r="F52">
-        <f t="shared" ca="1" si="1"/>
-        <v>99.326999999999998</v>
-      </c>
-      <c r="G52">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99.977000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -5303,15 +5123,10 @@
         <v>4.7689199999999996</v>
       </c>
       <c r="F53">
-        <f t="shared" ca="1" si="1"/>
-        <v>98.977000000000004</v>
-      </c>
-      <c r="G53">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99.927000000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -5330,12 +5145,7 @@
         <v>4.7689199999999996</v>
       </c>
       <c r="F54">
-        <f t="shared" ca="1" si="1"/>
-        <v>98.927000000000007</v>
-      </c>
-      <c r="G54">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.05</v>
+        <v>99.527000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -5349,7 +5159,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5821,209 +5631,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>